<commit_message>
Added data combined model experiment 1
</commit_message>
<xml_diff>
--- a/evaluations/OverviewExperiment1.xlsx
+++ b/evaluations/OverviewExperiment1.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Modell</t>
   </si>
@@ -67,6 +67,9 @@
   </si>
   <si>
     <t>Tan Quality Score</t>
+  </si>
+  <si>
+    <t>Combined Gemma Model</t>
   </si>
 </sst>
 </file>
@@ -399,10 +402,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -468,15 +471,15 @@
         <v>8.41</v>
       </c>
       <c r="D3">
-        <f t="shared" ref="D3:D12" si="0" xml:space="preserve"> -LOG(B3)</f>
+        <f t="shared" ref="D3:D13" si="0" xml:space="preserve"> -LOG(B3)</f>
         <v>1.7856399709145874</v>
       </c>
       <c r="E3">
-        <f t="shared" ref="E3:E12" si="1">TAN(3.14159265  * (  (C3 / 9)  - 11/18   )  )</f>
+        <f t="shared" ref="E3:E13" si="1">TAN(3.14159265  * (  (C3 / 9)  - 11/18   )  )</f>
         <v>1.6128348868108635</v>
       </c>
       <c r="F3">
-        <f t="shared" ref="F3:F12" si="2">E3 + D3</f>
+        <f t="shared" ref="F3:F13" si="2">E3 + D3</f>
         <v>3.3984748577254509</v>
       </c>
     </row>
@@ -686,6 +689,29 @@
       <c r="F12">
         <f t="shared" si="2"/>
         <v>4.3745562772852535</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13">
+        <v>6.4874064200000003E-3</v>
+      </c>
+      <c r="C13" s="1">
+        <v>8.94</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>2.1879288937401311</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="1"/>
+        <v>2.5781539047792075</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="2"/>
+        <v>4.7660827985193386</v>
       </c>
     </row>
   </sheetData>

</xml_diff>